<commit_message>
re-edit page view student
</commit_message>
<xml_diff>
--- a/import/list_group_1_TT.xlsx
+++ b/import/list_group_1_TT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\nckh_ng\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7097659B-1D93-40EB-A1E7-267C88AD1B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19995A88-4E21-4B9C-AB9A-87FC1FEB8C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0B75C513-079B-43B1-8E8C-1AF3886AC72B}"/>
   </bookViews>
@@ -327,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -350,21 +350,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -375,12 +360,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,6 +394,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,18 +737,18 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
     <col min="4" max="4" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -787,11 +772,11 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -801,11 +786,11 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -815,11 +800,11 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -829,11 +814,11 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -843,575 +828,575 @@
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>2</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>2</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5">
         <v>2</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>3</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="9">
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7">
         <v>3</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="9">
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7">
         <v>3</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+    <row r="16" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="9">
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="7">
         <v>3</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="9">
         <v>4</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="9">
         <v>4</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="11">
+      <c r="B19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9">
         <v>4</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="11">
+      <c r="B20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9">
         <v>4</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="11">
+      <c r="B21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="9">
         <v>4</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <v>5</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
+    <row r="23" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="11">
         <v>5</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+    <row r="24" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="13">
+      <c r="B24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="11">
         <v>5</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="13">
+      <c r="B25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="11">
         <v>5</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="13">
+      <c r="B26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="11">
         <v>5</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="13">
         <v>6</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="13">
         <v>6</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="15">
+      <c r="B29" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="13">
         <v>6</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="15">
+      <c r="B30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="13">
         <v>6</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="15">
+      <c r="B31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="13">
         <v>6</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="15">
         <v>7</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16" t="s">
+    <row r="33" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="15">
         <v>7</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="16" t="s">
+    <row r="34" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="17">
+      <c r="B34" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="15">
         <v>7</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="17">
+      <c r="B35" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="15">
         <v>7</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
+    <row r="36" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="17">
+      <c r="B36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="15">
         <v>7</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="17">
         <v>8</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="18" t="s">
+    <row r="38" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="17">
         <v>8</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="18" t="s">
+    <row r="39" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="19">
+      <c r="B39" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="17">
         <v>8</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="18" t="s">
+    <row r="40" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="19">
+      <c r="B40" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="17">
         <v>8</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="18" t="s">
+    <row r="41" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="19">
+      <c r="B41" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="17">
         <v>8</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="20" t="s">
+    <row r="42" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="21">
-        <v>9</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="C42" s="19">
+        <v>9</v>
+      </c>
+      <c r="D42" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="20" t="s">
+    <row r="43" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="21">
-        <v>9</v>
-      </c>
-      <c r="D43" s="5" t="s">
+      <c r="C43" s="19">
+        <v>9</v>
+      </c>
+      <c r="D43" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="20" t="s">
+    <row r="44" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="21">
-        <v>9</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="B44" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="19">
+        <v>9</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="20" t="s">
+    <row r="45" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="21">
-        <v>9</v>
-      </c>
-      <c r="D45" s="5" t="s">
+      <c r="B45" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="19">
+        <v>9</v>
+      </c>
+      <c r="D45" s="22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="20" t="s">
+    <row r="46" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="21">
-        <v>9</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="B46" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="19">
+        <v>9</v>
+      </c>
+      <c r="D46" s="21" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete show manager report
</commit_message>
<xml_diff>
--- a/import/list_group_1_TT.xlsx
+++ b/import/list_group_1_TT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\nckh_ng\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19995A88-4E21-4B9C-AB9A-87FC1FEB8C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D2B2CA-0379-47D6-B912-A15500E906EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0B75C513-079B-43B1-8E8C-1AF3886AC72B}"/>
   </bookViews>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F325DC-DB6E-4990-9EBE-C2F9E9152327}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>